<commit_message>
Correction to find_alternative_fans.py quick test conditions
</commit_message>
<xml_diff>
--- a/fan_database/sanyo denki_full.xlsx
+++ b/fan_database/sanyo denki_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoãoGonçaloCouto\PycharmProjects\fan_selector\fan_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7930D6F-DA61-4C90-A3FE-83388974BFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D27901-F2BB-41D7-A2FA-BA2F2D1B5DCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="-110" windowWidth="36560" windowHeight="21820" xr2:uid="{6B83A61E-00AF-40C2-B298-003C066BCD05}"/>
+    <workbookView xWindow="1650" yWindow="-110" windowWidth="36860" windowHeight="21820" xr2:uid="{6B83A61E-00AF-40C2-B298-003C066BCD05}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1559,7 +1559,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O320" sqref="O320"/>
+      <selection pane="bottomLeft" activeCell="K332" sqref="K332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19597,5 +19597,6 @@
     <hyperlink ref="C319" r:id="rId318" display="https://products.sanyodenki.com/en/sanace/dc/dc-fan/9GV0812P1F03/" xr:uid="{26D4979B-02A1-4F4F-A598-CD903E3B4193}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId319"/>
 </worksheet>
 </file>
</xml_diff>